<commit_message>
fix typos in section 6.
</commit_message>
<xml_diff>
--- a/Part_II/2_Data/Laser_Analysis.xlsx
+++ b/Part_II/2_Data/Laser_Analysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21640" yWindow="2660" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="23600" windowHeight="16400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -117,6 +117,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -158,10 +161,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P36"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -450,6 +456,7 @@
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -700,406 +707,498 @@
         <v>1.9666666666666666</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>0</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>20</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>21</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>2</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="3">
         <v>1.6706270000000001</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="3">
         <v>4.0921659999999997</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="3">
+        <f>C18-B18</f>
+        <v>2.4215389999999997</v>
+      </c>
+      <c r="E18" s="3">
         <v>4.0921659999999997</v>
       </c>
-      <c r="E18" s="2">
+      <c r="F18" s="3">
         <v>4.0921659999999997</v>
       </c>
-      <c r="F18" s="2">
+      <c r="G18" s="3">
         <v>4.0999999999999996</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="3">
+        <f>G18-B18</f>
+        <v>2.4293729999999996</v>
+      </c>
+      <c r="J18" t="s">
         <v>22</v>
       </c>
-      <c r="I18" t="s">
+      <c r="K18" t="s">
         <v>27</v>
       </c>
-      <c r="P18" t="s">
+      <c r="R18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="4">
         <v>1.0923639999999999</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="4">
         <v>4.4005809999999999</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="3">
+        <f t="shared" ref="D19:D29" si="4">C19-B19</f>
+        <v>3.308217</v>
+      </c>
+      <c r="E19" s="4">
         <v>4.9260169999999999</v>
       </c>
-      <c r="E19">
+      <c r="F19" s="4">
         <v>4.5821740000000002</v>
       </c>
-      <c r="F19">
+      <c r="G19" s="4">
         <v>5</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="3">
+        <f t="shared" ref="H19:H28" si="5">G19-B19</f>
+        <v>3.9076360000000001</v>
+      </c>
+      <c r="J19" t="s">
         <v>22</v>
       </c>
-      <c r="I19" t="s">
+      <c r="K19" t="s">
         <v>27</v>
       </c>
-      <c r="P19" t="s">
+      <c r="R19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="5">
         <v>1.67489971</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="5">
         <v>2.0042877059999999</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="3">
+        <f t="shared" si="4"/>
+        <v>0.32938799599999991</v>
+      </c>
+      <c r="E20" s="5">
         <v>4.3229469920000003</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="5">
         <v>4.3229469920000003</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G20" s="5">
         <v>5.5</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="3">
+        <f t="shared" si="5"/>
+        <v>3.82510029</v>
+      </c>
+      <c r="J20" t="s">
         <v>23</v>
       </c>
-      <c r="I20" t="s">
+      <c r="K20" t="s">
         <v>26</v>
       </c>
-      <c r="J20">
-        <f>D20-C20</f>
+      <c r="L20">
+        <f>E20-C20</f>
         <v>2.3186592860000004</v>
       </c>
-      <c r="P20" t="s">
+      <c r="R20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="3">
         <v>1.55591363</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="3">
         <v>4.8864029000000002</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="3">
+        <f t="shared" si="4"/>
+        <v>3.3304892700000002</v>
+      </c>
+      <c r="E21" s="3">
         <v>4.8864029000000002</v>
       </c>
-      <c r="E21" s="2">
+      <c r="F21" s="3">
         <v>4.8864029000000002</v>
       </c>
-      <c r="F21" s="2">
+      <c r="G21" s="3">
         <v>4</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="3">
+        <f t="shared" si="5"/>
+        <v>2.44408637</v>
+      </c>
+      <c r="J21" t="s">
         <v>22</v>
       </c>
-      <c r="I21" t="s">
+      <c r="K21" t="s">
         <v>25</v>
       </c>
-      <c r="P21" t="s">
+      <c r="R21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="3">
         <v>1.5418684170000001</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="3">
         <v>3.3729445149999999</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="3">
+        <f t="shared" si="4"/>
+        <v>1.8310760979999998</v>
+      </c>
+      <c r="E22" s="3">
         <v>3.7376470290000001</v>
       </c>
-      <c r="E22" s="2">
+      <c r="F22" s="3">
         <v>3.31205047</v>
       </c>
-      <c r="F22" s="2">
+      <c r="G22" s="3">
         <v>4</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="3">
+        <f t="shared" si="5"/>
+        <v>2.4581315830000001</v>
+      </c>
+      <c r="J22" t="s">
         <v>24</v>
       </c>
-      <c r="I22" t="s">
+      <c r="K22" t="s">
         <v>25</v>
       </c>
-      <c r="P22" t="s">
+      <c r="R22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>12</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="4">
         <v>0.85547399999999996</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="4">
         <v>1.073318</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.21784400000000004</v>
+      </c>
+      <c r="E23" s="4">
         <v>1.1997249999999999</v>
       </c>
-      <c r="E23">
+      <c r="F23" s="4">
         <v>1.2631049999999999</v>
       </c>
-      <c r="F23">
+      <c r="G23" s="4">
         <v>2</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="3">
+        <f t="shared" si="5"/>
+        <v>1.1445259999999999</v>
+      </c>
+      <c r="J23" t="s">
         <v>22</v>
       </c>
-      <c r="I23" t="s">
+      <c r="K23" t="s">
         <v>26</v>
       </c>
-      <c r="P23" t="s">
+      <c r="R23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>13</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="4">
         <v>1.38188</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="4">
         <v>1.1422920000000001</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.23958799999999991</v>
+      </c>
+      <c r="E24" s="4">
         <v>1.8559779999999999</v>
       </c>
-      <c r="E24">
+      <c r="F24" s="4">
         <v>1.826114</v>
       </c>
-      <c r="F24">
+      <c r="G24" s="4">
         <v>3.3</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="3">
+        <f t="shared" si="5"/>
+        <v>1.9181199999999998</v>
+      </c>
+      <c r="J24" t="s">
         <v>22</v>
       </c>
-      <c r="I24" t="s">
+      <c r="K24" t="s">
         <v>26</v>
       </c>
-      <c r="P24" t="s">
+      <c r="R24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>14</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="4">
         <v>1.957452789</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="4">
         <v>2.169149778</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="3">
+        <f t="shared" si="4"/>
+        <v>0.211696989</v>
+      </c>
+      <c r="E25" s="4">
         <v>4.3987701250000004</v>
       </c>
-      <c r="E25">
+      <c r="F25" s="4">
         <v>5.0202826580000002</v>
       </c>
-      <c r="F25">
+      <c r="G25" s="4">
         <v>5.7</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="3">
+        <f t="shared" si="5"/>
+        <v>3.7425472110000002</v>
+      </c>
+      <c r="J25" t="s">
         <v>22</v>
       </c>
-      <c r="I25" t="s">
+      <c r="K25" t="s">
         <v>26</v>
       </c>
-      <c r="P25" t="s">
+      <c r="R25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="5">
         <v>2.1829094320000002</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="5">
         <v>5.0287161630000003</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="3">
+        <f t="shared" si="4"/>
+        <v>2.8458067310000001</v>
+      </c>
+      <c r="E26" s="5">
         <v>5.5219787289999998</v>
       </c>
-      <c r="E26" s="1">
+      <c r="F26" s="5">
         <v>6.3384754970000001</v>
       </c>
-      <c r="F26" s="1">
+      <c r="G26" s="5">
         <v>9.1</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="3">
+        <f t="shared" si="5"/>
+        <v>6.917090567999999</v>
+      </c>
+      <c r="J26" t="s">
         <v>23</v>
       </c>
-      <c r="I26" t="s">
+      <c r="K26" t="s">
         <v>26</v>
       </c>
-      <c r="J26">
-        <f>D26-C26</f>
+      <c r="L26">
+        <f>E26-C26</f>
         <v>0.4932625659999994</v>
       </c>
-      <c r="P26" t="s">
+      <c r="R26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="3">
         <v>1.636236647</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="3">
         <v>4.6847521810000003</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="3">
+        <f t="shared" si="4"/>
+        <v>3.0485155340000003</v>
+      </c>
+      <c r="E27" s="3">
         <v>4.6847521810000003</v>
       </c>
-      <c r="E27" s="2">
+      <c r="F27" s="3">
         <v>5.6222523989999997</v>
       </c>
-      <c r="F27" s="2">
+      <c r="G27" s="3">
         <v>6.8</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="3">
+        <f t="shared" si="5"/>
+        <v>5.1637633530000002</v>
+      </c>
+      <c r="J27" t="s">
         <v>23</v>
       </c>
-      <c r="I27" t="s">
+      <c r="K27" t="s">
         <v>26</v>
       </c>
-      <c r="P27" t="s">
+      <c r="R27" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="5">
         <v>2.170718908</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="5">
         <v>4.4314430319999998</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="3">
+        <f t="shared" si="4"/>
+        <v>2.2607241239999998</v>
+      </c>
+      <c r="E28" s="5">
         <v>6.7355238110000002</v>
       </c>
-      <c r="E28" s="1">
+      <c r="F28" s="5">
         <v>7.6325335340000002</v>
       </c>
-      <c r="F28" s="1">
+      <c r="G28" s="5">
         <v>8</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" s="3">
+        <f t="shared" si="5"/>
+        <v>5.8292810920000004</v>
+      </c>
+      <c r="J28" t="s">
         <v>23</v>
       </c>
-      <c r="I28" t="s">
+      <c r="K28" t="s">
         <v>26</v>
       </c>
-      <c r="J28">
-        <f>D28-C28</f>
+      <c r="L28">
+        <f>E28-C28</f>
         <v>2.3040807790000004</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>3</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="4">
         <f>AVERAGE(B23:B25,B19)</f>
         <v>1.3217926972499998</v>
       </c>
-      <c r="C29">
-        <f t="shared" ref="C29:F29" si="4">AVERAGE(C23:C25,C19)</f>
+      <c r="C29" s="4">
+        <f t="shared" ref="C29:G29" si="6">AVERAGE(C23:C25,C19)</f>
         <v>2.1963351944999996</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="3">
         <f t="shared" si="4"/>
+        <v>0.87454249724999977</v>
+      </c>
+      <c r="E29" s="4">
+        <f t="shared" si="6"/>
         <v>3.0951225312499999</v>
       </c>
-      <c r="E29">
-        <f t="shared" si="4"/>
+      <c r="F29" s="4">
+        <f t="shared" si="6"/>
         <v>3.1729189144999999</v>
       </c>
-      <c r="F29">
-        <f t="shared" si="4"/>
+      <c r="G29" s="4">
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="G29">
-        <f>C29-B29</f>
-        <v>0.87454249724999977</v>
-      </c>
-      <c r="H29">
-        <f>F29-C29</f>
+      <c r="H29" s="4">
+        <f>AVERAGE(H18:H28)</f>
+        <v>3.6163323151818179</v>
+      </c>
+      <c r="I29">
+        <f>G29-C29</f>
         <v>1.8036648055000004</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B30">
         <f>AVERAGE(B26:B28,B20)</f>
         <v>1.9161911742500002</v>
       </c>
       <c r="C30">
-        <f t="shared" ref="C30:F30" si="5">AVERAGE(C26:C28,C20)</f>
+        <f t="shared" ref="C30" si="7">AVERAGE(C26:C28,C20)</f>
         <v>4.0372997704999998</v>
       </c>
       <c r="D30">
-        <f t="shared" si="5"/>
+        <f>AVERAGE(E26:E28,E20)</f>
         <v>5.3163004282500008</v>
       </c>
       <c r="E30">
-        <f t="shared" si="5"/>
+        <f>AVERAGE(F26:F28,F20)</f>
         <v>5.9790521054999992</v>
       </c>
       <c r="F30">
-        <f t="shared" si="5"/>
+        <f>AVERAGE(G26:G28,G20)</f>
         <v>7.35</v>
       </c>
       <c r="G30">
@@ -1111,7 +1210,7 @@
         <v>3.3127002294999999</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -1120,19 +1219,19 @@
         <v>1.5071345513999999</v>
       </c>
       <c r="C31">
-        <f t="shared" ref="C31:F31" si="6">AVERAGE(C18:C22)</f>
+        <f t="shared" ref="C31" si="8">AVERAGE(C18:C22)</f>
         <v>3.7512764241999994</v>
       </c>
       <c r="D31">
-        <f t="shared" si="6"/>
+        <f>AVERAGE(E18:E22)</f>
         <v>4.3930359842</v>
       </c>
       <c r="E31">
-        <f>AVERAGE(E18:E22)</f>
+        <f>AVERAGE(F18:F22)</f>
         <v>4.2391480723999999</v>
       </c>
       <c r="F31">
-        <f t="shared" si="6"/>
+        <f>AVERAGE(G18:G22)</f>
         <v>4.5200000000000005</v>
       </c>
       <c r="G31">
@@ -1144,7 +1243,7 @@
         <v>0.76872357580000106</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -1153,19 +1252,19 @@
         <v>1.3982689296666664</v>
       </c>
       <c r="C32">
-        <f t="shared" ref="C32:F32" si="7">AVERAGE(C23:C25)</f>
+        <f t="shared" ref="C32" si="9">AVERAGE(C23:C25)</f>
         <v>1.4615865926666665</v>
       </c>
       <c r="D32">
-        <f t="shared" si="7"/>
+        <f>AVERAGE(E23:E25)</f>
         <v>2.4848243750000001</v>
       </c>
       <c r="E32">
-        <f>AVERAGE(E23:E25)</f>
+        <f>AVERAGE(F23:F25)</f>
         <v>2.7031672193333329</v>
       </c>
       <c r="F32">
-        <f t="shared" si="7"/>
+        <f>AVERAGE(G23:G25)</f>
         <v>3.6666666666666665</v>
       </c>
       <c r="G32">
@@ -1177,38 +1276,60 @@
         <v>2.2050800740000001</v>
       </c>
     </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C34">
         <f>C29-B29</f>
         <v>0.87454249724999977</v>
       </c>
       <c r="D34">
-        <f>D29-C29</f>
+        <f>E29-C29</f>
         <v>0.89878733675000033</v>
       </c>
       <c r="E34">
-        <f>E29-C29</f>
+        <f>F29-C29</f>
         <v>0.97658372000000027</v>
       </c>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
       <c r="D35">
-        <f t="shared" ref="D35:D36" si="8">D31-C31</f>
+        <f t="shared" ref="D35:D36" si="10">D31-C31</f>
         <v>0.64175956000000056</v>
       </c>
       <c r="E35">
-        <f t="shared" ref="E35:E36" si="9">E31-C31</f>
+        <f t="shared" ref="E35:E36" si="11">E31-C31</f>
         <v>0.48787164820000051</v>
       </c>
     </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
       <c r="D36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.0232377823333336</v>
       </c>
       <c r="E36">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.2415806266666665</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B38">
+        <f>_xlfn.STDEV.P(B18:B28)</f>
+        <v>0.38949653823295172</v>
+      </c>
+      <c r="C38">
+        <f>_xlfn.STDEV.P(C18:C28)</f>
+        <v>1.446942864752101</v>
+      </c>
+      <c r="D38">
+        <f>_xlfn.STDEV.P(D18:D28)</f>
+        <v>1.3215938921787043</v>
+      </c>
+      <c r="G38">
+        <f>_xlfn.STDEV.P(G18:G28)</f>
+        <v>1.9982223504864203</v>
+      </c>
+      <c r="H38">
+        <f>_xlfn.STDEV.P(H18:H28)</f>
+        <v>1.6908651816673019</v>
       </c>
     </row>
   </sheetData>

</xml_diff>